<commit_message>
block message checking added
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -40,18 +40,68 @@
   </si>
   <si>
     <t>PROXY_PASS</t>
+  </si>
+  <si>
+    <t>Anastasia</t>
+  </si>
+  <si>
+    <t>Jimenez</t>
+  </si>
+  <si>
+    <t>Anastasia.Jimenez1990@gmail.com</t>
+  </si>
+  <si>
+    <t>R4ehM6vA8xtaDpwm</t>
+  </si>
+  <si>
+    <t>81.28.96.172:41489</t>
+  </si>
+  <si>
+    <t>a4ZJCKXpyPxqtgAt</t>
+  </si>
+  <si>
+    <t>WZRYymEeVjfQeR6Z</t>
+  </si>
+  <si>
+    <t>23.94.179.27:1311</t>
+  </si>
+  <si>
+    <t>tqD6fggLah4JM24d</t>
+  </si>
+  <si>
+    <t>SLfNnLB2fbV9s4NX</t>
+  </si>
+  <si>
+    <t>Martina</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Martina.gramdominator@gmail.com</t>
+  </si>
+  <si>
+    <t>Ekmyd38VrWUTZnGM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -181,6 +231,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -363,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -478,53 +536,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -846,11 +926,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -875,7 +962,54 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added linebreak in utils.format_email()
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -40,6 +40,42 @@
   </si>
   <si>
     <t>PROXY_PASS</t>
+  </si>
+  <si>
+    <t>Elva</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Elva.Lynn1987@gmail.com</t>
+  </si>
+  <si>
+    <t>C9nqK4Xz6gbUocjf</t>
+  </si>
+  <si>
+    <t>81.28.96.172:43739</t>
+  </si>
+  <si>
+    <t>a4ZJCKXpyPxqtgAt</t>
+  </si>
+  <si>
+    <t>WZRYymEeVjfQeR6Z</t>
+  </si>
+  <si>
+    <t>Daphne</t>
+  </si>
+  <si>
+    <t>Boone</t>
+  </si>
+  <si>
+    <t>Daphne.Boone2002@gmail.com</t>
+  </si>
+  <si>
+    <t>aPxbySqRts82761Y</t>
+  </si>
+  <si>
+    <t>81.28.96.172:30660</t>
   </si>
 </sst>
 </file>
@@ -182,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,12 +396,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -529,9 +559,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="A2:H29"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,23 +947,51 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
separated database file loading and fixed header problem while loading file
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Upwork\2020\gmail_app\gmail_app\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GMonster\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="group_b" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -42,47 +42,275 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t>Elva</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Elva.Lynn1987@gmail.com</t>
-  </si>
-  <si>
-    <t>C9nqK4Xz6gbUocjf</t>
-  </si>
-  <si>
-    <t>81.28.96.172:43739</t>
-  </si>
-  <si>
-    <t>a4ZJCKXpyPxqtgAt</t>
-  </si>
-  <si>
-    <t>WZRYymEeVjfQeR6Z</t>
-  </si>
-  <si>
-    <t>Daphne</t>
-  </si>
-  <si>
-    <t>Boone</t>
-  </si>
-  <si>
-    <t>Daphne.Boone2002@gmail.com</t>
-  </si>
-  <si>
-    <t>aPxbySqRts82761Y</t>
-  </si>
-  <si>
-    <t>81.28.96.172:30660</t>
+    <t>nandapdinht@gmail.com</t>
+  </si>
+  <si>
+    <t>Seslought</t>
+  </si>
+  <si>
+    <t>Lithoathea</t>
+  </si>
+  <si>
+    <t>857gkyai857</t>
+  </si>
+  <si>
+    <t>81.28.96.131:4013</t>
+  </si>
+  <si>
+    <t>kMp298uK9PLMARGv</t>
+  </si>
+  <si>
+    <t>XEErfk67umzgWC5d</t>
+  </si>
+  <si>
+    <t>Thoaneni</t>
+  </si>
+  <si>
+    <t>Litethannit</t>
+  </si>
+  <si>
+    <t>vanitabdaoib@gmail.com</t>
+  </si>
+  <si>
+    <t>491pmwbh491</t>
+  </si>
+  <si>
+    <t>Sepasheaus</t>
+  </si>
+  <si>
+    <t>Smoughshes</t>
+  </si>
+  <si>
+    <t>jaladhicnxyhd@gmail.com</t>
+  </si>
+  <si>
+    <t>719uaywr719</t>
+  </si>
+  <si>
+    <t>Seslatileaus</t>
+  </si>
+  <si>
+    <t>Pheteighse</t>
+  </si>
+  <si>
+    <t>ganithaiwkkya@gmail.com</t>
+  </si>
+  <si>
+    <t>275qzcjf275</t>
+  </si>
+  <si>
+    <t>Wosethay</t>
+  </si>
+  <si>
+    <t>Sheammawheau</t>
+  </si>
+  <si>
+    <t>elilixkbdqi@gmail.com</t>
+  </si>
+  <si>
+    <t>930jxdyp930</t>
+  </si>
+  <si>
+    <t>Neenethoki</t>
+  </si>
+  <si>
+    <t>Thilleaslough</t>
+  </si>
+  <si>
+    <t>upasanacvlsce@gmail.com</t>
+  </si>
+  <si>
+    <t>732yoefp732</t>
+  </si>
+  <si>
+    <t>Deamuwethe</t>
+  </si>
+  <si>
+    <t>Setithough</t>
+  </si>
+  <si>
+    <t>safialjakgy@gmail.com</t>
+  </si>
+  <si>
+    <t>520roukm520</t>
+  </si>
+  <si>
+    <t>Titysen</t>
+  </si>
+  <si>
+    <t>Roathetethea</t>
+  </si>
+  <si>
+    <t>upamalrzaje@gmail.com</t>
+  </si>
+  <si>
+    <t>639pdkhr639</t>
+  </si>
+  <si>
+    <t>Smesaythay</t>
+  </si>
+  <si>
+    <t>Sasoaseed</t>
+  </si>
+  <si>
+    <t>achalafxdetu@gmail.com</t>
+  </si>
+  <si>
+    <t>365wekfj365</t>
+  </si>
+  <si>
+    <t>Styslena</t>
+  </si>
+  <si>
+    <t>Setasegen</t>
+  </si>
+  <si>
+    <t>haripriyaxtuqcw@gmail.com</t>
+  </si>
+  <si>
+    <t>265hznel265</t>
+  </si>
+  <si>
+    <t>Thashare</t>
+  </si>
+  <si>
+    <t>Shithesho</t>
+  </si>
+  <si>
+    <t>sagarikaoeptbh@gmail.com</t>
+  </si>
+  <si>
+    <t>561acrsd561</t>
+  </si>
+  <si>
+    <t>81.28.96.131:4022</t>
+  </si>
+  <si>
+    <t>Steteasa</t>
+  </si>
+  <si>
+    <t>Teadarrou</t>
+  </si>
+  <si>
+    <t>indiyafmpfnp@gmail.com</t>
+  </si>
+  <si>
+    <t>196gtpxt196</t>
+  </si>
+  <si>
+    <t>Thesathit</t>
+  </si>
+  <si>
+    <t>Quisethou</t>
+  </si>
+  <si>
+    <t>taptibpvlqs@gmail.com</t>
+  </si>
+  <si>
+    <t>468rzjpk468</t>
+  </si>
+  <si>
+    <t>Peighdyneath</t>
+  </si>
+  <si>
+    <t>Faysaseau</t>
+  </si>
+  <si>
+    <t>mahadeviwzuyfa@gmail.com</t>
+  </si>
+  <si>
+    <t>215bhitu215</t>
+  </si>
+  <si>
+    <t>Steslaseesm</t>
+  </si>
+  <si>
+    <t>Thasheythoa</t>
+  </si>
+  <si>
+    <t>sachiniqklefp@gmail.com</t>
+  </si>
+  <si>
+    <t>875padhw875</t>
+  </si>
+  <si>
+    <t>Tanaysetou</t>
+  </si>
+  <si>
+    <t>Thetheteighs</t>
+  </si>
+  <si>
+    <t>chanchalajmepfh@gmail.com</t>
+  </si>
+  <si>
+    <t>839dfxqd839</t>
+  </si>
+  <si>
+    <t>Netoashu</t>
+  </si>
+  <si>
+    <t>Datetode</t>
+  </si>
+  <si>
+    <t>tanukagvaodx@gmail.com</t>
+  </si>
+  <si>
+    <t>216fykvu216</t>
+  </si>
+  <si>
+    <t>Slasoushea</t>
+  </si>
+  <si>
+    <t>Thothaytha</t>
+  </si>
+  <si>
+    <t>elavarasicvlqjv@gmail.com</t>
+  </si>
+  <si>
+    <t>197tfeca197</t>
+  </si>
+  <si>
+    <t>Sheyrira</t>
+  </si>
+  <si>
+    <t>Neesesasheigh</t>
+  </si>
+  <si>
+    <t>panchalikjuvdh@gmail.com</t>
+  </si>
+  <si>
+    <t>648eyiuc648</t>
+  </si>
+  <si>
+    <t>Soaseywhy</t>
+  </si>
+  <si>
+    <t>Roulytythet</t>
+  </si>
+  <si>
+    <t>gangikarzfjqk@gmail.com</t>
+  </si>
+  <si>
+    <t>807zixkr807</t>
+  </si>
+  <si>
+    <t>Mootheteden</t>
+  </si>
+  <si>
+    <t>Taysheslou</t>
+  </si>
+  <si>
+    <t>adarshaphfedi@gmail.com</t>
+  </si>
+  <si>
+    <t>206dbksy206</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,7 +372,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,6 +445,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -399,7 +650,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -514,8 +765,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -537,32 +803,41 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -600,6 +875,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -636,7 +912,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -648,7 +924,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -665,9 +941,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -695,31 +971,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -747,23 +1006,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -916,15 +1158,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -947,17 +1196,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
@@ -970,30 +1219,488 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
user keyword check_for_blocks related problem solved
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="157">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -42,574 +42,454 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t>Adele</t>
-  </si>
-  <si>
-    <t>Putnam</t>
-  </si>
-  <si>
-    <t>adeleputnam310@gmail.com</t>
-  </si>
-  <si>
-    <t>glvopwtgimoycuhr</t>
-  </si>
-  <si>
-    <t>194.32.107.161:59028</t>
-  </si>
-  <si>
-    <t>rXdE4qNXsXXwpyvD</t>
-  </si>
-  <si>
-    <t>qD8wKTgE9UEGa4BH</t>
-  </si>
-  <si>
-    <t>Melany</t>
-  </si>
-  <si>
-    <t>Moss</t>
-  </si>
-  <si>
-    <t>melanymoss86@gmail.com</t>
-  </si>
-  <si>
-    <t>mtuovclngjmudqiu</t>
-  </si>
-  <si>
-    <t>194.32.107.161:35957</t>
-  </si>
-  <si>
-    <t>Khalilah</t>
-  </si>
-  <si>
-    <t>Hope</t>
-  </si>
-  <si>
-    <t>hopekhalilah110@gmail.com</t>
-  </si>
-  <si>
-    <t>kfgnynluosdzdiyd</t>
-  </si>
-  <si>
-    <t>81.28.96.144:8595</t>
-  </si>
-  <si>
-    <t>QLkhv5HXmsbU8qNU</t>
-  </si>
-  <si>
-    <t>Zx42Jx5vJ2ekAWWT</t>
-  </si>
-  <si>
     <t>Angela</t>
   </si>
   <si>
-    <t>Coffman</t>
-  </si>
-  <si>
-    <t>angelacoffman453@gmail.com</t>
-  </si>
-  <si>
-    <t>igansnutkdalgjmo</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4013</t>
-  </si>
-  <si>
-    <t>8GbKtEpRUr29jbg5</t>
-  </si>
-  <si>
-    <t>TMwprA4NyqSKxc6V</t>
-  </si>
-  <si>
-    <t>Joie</t>
-  </si>
-  <si>
-    <t>Hacker</t>
-  </si>
-  <si>
-    <t>joiehacker719@gmail.com</t>
-  </si>
-  <si>
-    <t>loehjsctdwfweaii</t>
-  </si>
-  <si>
-    <t>23.94.96.119:3168</t>
-  </si>
-  <si>
-    <t>6TFkNpfJJP2mVJ27</t>
-  </si>
-  <si>
-    <t>98hyShw5PC9D2vgw</t>
-  </si>
-  <si>
-    <t>Amber</t>
-  </si>
-  <si>
-    <t>Vick</t>
-  </si>
-  <si>
-    <t>ambervick53@gmail.com</t>
-  </si>
-  <si>
-    <t>bixkrynalikpzbkz</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4003</t>
-  </si>
-  <si>
-    <t>Karri</t>
-  </si>
-  <si>
-    <t>Rush</t>
-  </si>
-  <si>
-    <t>krush4092@gmail.com</t>
-  </si>
-  <si>
-    <t>mknsqodtqoaixsnk</t>
-  </si>
-  <si>
-    <t>103.144.176.25:4002</t>
-  </si>
-  <si>
-    <t>7rcmKcMRkAx4NgzX</t>
-  </si>
-  <si>
-    <t>sGVYb9mGA92MZ9TQ</t>
-  </si>
-  <si>
-    <t>Loralee</t>
-  </si>
-  <si>
-    <t>Rhodes</t>
-  </si>
-  <si>
-    <t>rhodesloralee@gmail.com</t>
-  </si>
-  <si>
-    <t>hzjuozklbpcjanhn</t>
-  </si>
-  <si>
-    <t>23.94.96.119:3169</t>
-  </si>
-  <si>
-    <t>Kathryne</t>
-  </si>
-  <si>
-    <t>Pruett</t>
-  </si>
-  <si>
-    <t>kathrynepruett@gmail.com</t>
-  </si>
-  <si>
-    <t>eyzfclhtixzwojed</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4015</t>
-  </si>
-  <si>
-    <t>Maribeth</t>
-  </si>
-  <si>
-    <t>Mckenna</t>
-  </si>
-  <si>
-    <t>maribeth884299mckenna884299@gmail.com</t>
-  </si>
-  <si>
-    <t>mfnivjuvwxycifyu</t>
-  </si>
-  <si>
-    <t>194.32.107.208:4031</t>
-  </si>
-  <si>
-    <t>PLacRXQmA8XV277b</t>
-  </si>
-  <si>
-    <t>t475U4Qqj7b9CbB2</t>
-  </si>
-  <si>
-    <t>Shanna</t>
-  </si>
-  <si>
-    <t>Burch</t>
-  </si>
-  <si>
-    <t>burchshanna603@gmail.com</t>
-  </si>
-  <si>
-    <t>rclvjbtxowduupsp</t>
-  </si>
-  <si>
-    <t>81.28.96.80:4011</t>
-  </si>
-  <si>
-    <t>ufp4gZaYukjRWNGH</t>
-  </si>
-  <si>
-    <t>7hyt5TpfptCKFgb5</t>
-  </si>
-  <si>
-    <t>Peg</t>
-  </si>
-  <si>
-    <t>Dorsey</t>
-  </si>
-  <si>
-    <t>pegdorsey88@gmail.com</t>
-  </si>
-  <si>
-    <t>diuflmbusvquppwk</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4001</t>
-  </si>
-  <si>
-    <t>Le</t>
-  </si>
-  <si>
-    <t>Ramsey</t>
-  </si>
-  <si>
-    <t>ramseyle445@gmail.com</t>
-  </si>
-  <si>
-    <t>jahgygfvlbebtrth</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4004</t>
-  </si>
-  <si>
-    <t>An</t>
-  </si>
-  <si>
-    <t>Jensen</t>
-  </si>
-  <si>
-    <t>an521633jensen521633@gmail.com</t>
-  </si>
-  <si>
-    <t>yilkxyjrtrfxswvr</t>
-  </si>
-  <si>
-    <t>194.32.107.51:4003</t>
-  </si>
-  <si>
-    <t>S6UxGStsBGjNnZ9c</t>
-  </si>
-  <si>
-    <t>HhL5TD4YwYRDZJFz</t>
-  </si>
-  <si>
-    <t>Florene</t>
-  </si>
-  <si>
-    <t>Smallwood</t>
-  </si>
-  <si>
-    <t>florenesmallwood54@gmail.com</t>
-  </si>
-  <si>
-    <t>awvpznmudlciciir</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4012</t>
-  </si>
-  <si>
-    <t>Julee</t>
-  </si>
-  <si>
-    <t>Sykes</t>
-  </si>
-  <si>
-    <t>sykesjulee530@gmail.com</t>
-  </si>
-  <si>
-    <t>fbxwgljoudcbpayn</t>
-  </si>
-  <si>
-    <t>194.32.107.85:4033</t>
-  </si>
-  <si>
-    <t>Am4qH9WTM5yr9NaY</t>
-  </si>
-  <si>
-    <t>8NrJvRAujAmcvtq7</t>
-  </si>
-  <si>
-    <t>Yvette</t>
-  </si>
-  <si>
-    <t>Ortiz</t>
-  </si>
-  <si>
-    <t>yo227241@gmail.com</t>
-  </si>
-  <si>
-    <t>zbkqgpuitaxjmexi</t>
-  </si>
-  <si>
-    <t>81.28.96.145:4003</t>
-  </si>
-  <si>
-    <t>KpbXsNM7RkxsXfWr</t>
-  </si>
-  <si>
-    <t>JYTtYbv6hPvJSqZc</t>
-  </si>
-  <si>
-    <t>Leona</t>
-  </si>
-  <si>
-    <t>Bateman</t>
-  </si>
-  <si>
-    <t>leonabateman7@gmail.com</t>
-  </si>
-  <si>
-    <t>fvngqzvdstlebstg</t>
-  </si>
-  <si>
-    <t>194.32.107.85:4034</t>
-  </si>
-  <si>
-    <t>Exie</t>
-  </si>
-  <si>
-    <t>Edmonds</t>
-  </si>
-  <si>
-    <t>exieedmonds@gmail.com</t>
-  </si>
-  <si>
-    <t>mhkvqoehnuqcyiem</t>
-  </si>
-  <si>
-    <t>Kristal</t>
-  </si>
-  <si>
-    <t>Abraham</t>
-  </si>
-  <si>
-    <t>krstlabraham@gmail.com</t>
-  </si>
-  <si>
-    <t>nbiyasmauoxdiaul</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4010</t>
-  </si>
-  <si>
-    <t>Liz</t>
-  </si>
-  <si>
     <t>Ruth</t>
   </si>
   <si>
-    <t>rliz20897@gmail.com</t>
-  </si>
-  <si>
-    <t>rsrjdcmthbyoioaj</t>
-  </si>
-  <si>
-    <t>Sherilyn</t>
-  </si>
-  <si>
-    <t>Collier</t>
-  </si>
-  <si>
-    <t>sherilync223@gmail.com</t>
-  </si>
-  <si>
-    <t>tewnhbzqknkykldr</t>
-  </si>
-  <si>
-    <t>Huong</t>
-  </si>
-  <si>
-    <t>Roth</t>
-  </si>
-  <si>
-    <t>rothhuong99@gmail.com</t>
-  </si>
-  <si>
-    <t>uguykpotcetxravn</t>
-  </si>
-  <si>
-    <t>81.28.96.145:4004</t>
-  </si>
-  <si>
-    <t>Pamala</t>
-  </si>
-  <si>
-    <t>Creech</t>
-  </si>
-  <si>
-    <t>pamalacreech58@gmail.com</t>
-  </si>
-  <si>
-    <t>dmlmfuwsjtocwabu</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4011</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>Garber</t>
-  </si>
-  <si>
-    <t>garberp108@gmail.com</t>
-  </si>
-  <si>
-    <t>zcsejoudmhlqijon</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4002</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>Bauer</t>
-  </si>
-  <si>
-    <t>jean13822bauer13822@gmail.com</t>
-  </si>
-  <si>
-    <t>aepislshmakxadqj</t>
-  </si>
-  <si>
-    <t>Georgann</t>
-  </si>
-  <si>
-    <t>Reese</t>
-  </si>
-  <si>
-    <t>georgannreese5@gmail.com</t>
-  </si>
-  <si>
-    <t>wdkzvbujfilbwtpz</t>
-  </si>
-  <si>
-    <t>Neta</t>
-  </si>
-  <si>
-    <t>Reardon</t>
-  </si>
-  <si>
-    <t>netareardon90@gmail.com</t>
-  </si>
-  <si>
-    <t>zhgsvidbwqmdczif</t>
-  </si>
-  <si>
-    <t>Young</t>
-  </si>
-  <si>
-    <t>Hendrix</t>
-  </si>
-  <si>
-    <t>hendrixy34@gmail.com</t>
-  </si>
-  <si>
-    <t>tuyabdllwufsbksf</t>
-  </si>
-  <si>
-    <t>Paulina</t>
-  </si>
-  <si>
-    <t>Workman</t>
-  </si>
-  <si>
-    <t>paulina82899workman82899@gmail.com</t>
-  </si>
-  <si>
-    <t>hwjlrpwgbwnzhrqd</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>Waddell</t>
-  </si>
-  <si>
-    <t>leewaddell239@gmail.com</t>
-  </si>
-  <si>
-    <t>fvkkfuqoaxlkugaf</t>
-  </si>
-  <si>
-    <t>Dorinda</t>
-  </si>
-  <si>
-    <t>Goldstein</t>
-  </si>
-  <si>
-    <t>goldsteindorinda30@gmail.com</t>
-  </si>
-  <si>
-    <t>rthwtbcufanfprdz</t>
-  </si>
-  <si>
-    <t>Lucienne</t>
-  </si>
-  <si>
-    <t>Graves</t>
-  </si>
-  <si>
-    <t>lucienne353002graves353002@gmail.com</t>
-  </si>
-  <si>
-    <t>cbbvucwnpcvfwtdx</t>
-  </si>
-  <si>
-    <t>Lynda</t>
-  </si>
-  <si>
-    <t>Giordano</t>
-  </si>
-  <si>
-    <t>giordanolynda2@gmail.com</t>
-  </si>
-  <si>
-    <t>sxdfceedmlrprgdy</t>
-  </si>
-  <si>
-    <t>Zelma</t>
-  </si>
-  <si>
-    <t>Aldrich</t>
-  </si>
-  <si>
-    <t>zelmaaldrich@gmail.com</t>
-  </si>
-  <si>
-    <t>vhshhmmmxqqcescz</t>
-  </si>
-  <si>
-    <t>Suzy</t>
-  </si>
-  <si>
-    <t>Rivera</t>
-  </si>
-  <si>
-    <t>riverasuzy635@gmail.com</t>
-  </si>
-  <si>
-    <t>bndmsyounuuhkizu</t>
-  </si>
-  <si>
-    <t>Vi</t>
-  </si>
-  <si>
-    <t>Stuart</t>
-  </si>
-  <si>
-    <t>vi262859stuart262859@gmail.com</t>
-  </si>
-  <si>
-    <t>zwbaiaqfwrqkanay</t>
+    <t>Teresa</t>
+  </si>
+  <si>
+    <t>Simmons</t>
+  </si>
+  <si>
+    <t>Teresasimmonsy3@gmail.com</t>
+  </si>
+  <si>
+    <t>kvnycktougwbblbi</t>
+  </si>
+  <si>
+    <t>23.152.224.240:24466</t>
+  </si>
+  <si>
+    <t>YU5E5Aj4nGuDgc9r</t>
+  </si>
+  <si>
+    <t>vn6hT75zxubw2FES</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Oliviadouglasy2@gmail.com</t>
+  </si>
+  <si>
+    <t>gxxjnmpzfghrllyg</t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Christinaoliveru3@gmail.com</t>
+  </si>
+  <si>
+    <t>wvlozcsowtsiiqjt</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>Christinaschneidery4@gmail.com</t>
+  </si>
+  <si>
+    <t>oplfrvbsriadcpag</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Barbararodriguezc4@gmail.com</t>
+  </si>
+  <si>
+    <t>jawidmafbhzdbrok</t>
+  </si>
+  <si>
+    <t>Katherine</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Katherinethomasc4@gmail.com</t>
+  </si>
+  <si>
+    <t>tjfmfzaylsxaovyy</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Jenniferhallc4@gmail.com</t>
+  </si>
+  <si>
+    <t>mbekqifkpbvjilea</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Annamayh3@gmail.com</t>
+  </si>
+  <si>
+    <t>qsjpuedpcygapdsj</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Barbaralopezv5@gmail.com</t>
+  </si>
+  <si>
+    <t>dckdayhpyhuarqrd</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Lauraharveyc3@gmail.com</t>
+  </si>
+  <si>
+    <t>fyvwhkhbkwkuehoo</t>
+  </si>
+  <si>
+    <t>23.152.224.240:2375</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Nicoleruizg4@gmail.com</t>
+  </si>
+  <si>
+    <t>gfarjtrrgszavpvt</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Sanders</t>
+  </si>
+  <si>
+    <t>Gracesandersy4@gmail.com</t>
+  </si>
+  <si>
+    <t>lnmckhsyqjesdous</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Melissatayloru3@gmail.com</t>
+  </si>
+  <si>
+    <t>bpkjejqbwmmhouqo</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Catherinewilliamsg3@gmail.com</t>
+  </si>
+  <si>
+    <t>jtxrwnyxuxyfnhxc</t>
+  </si>
+  <si>
+    <t>Cynthia</t>
+  </si>
+  <si>
+    <t>Ferguson</t>
+  </si>
+  <si>
+    <t>Cynthiafergusonx3@gmail.com</t>
+  </si>
+  <si>
+    <t>ckybtpwpzagpskfa</t>
+  </si>
+  <si>
+    <t>Griffin</t>
+  </si>
+  <si>
+    <t>Ruthgriffiny4@gmail.com</t>
+  </si>
+  <si>
+    <t>iylzusjhrupelnxq</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>barbaraknightx4@gmail.com</t>
+  </si>
+  <si>
+    <t>fzbgptuhzvnczweq</t>
+  </si>
+  <si>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Donnamorganv6@gmail.com</t>
+  </si>
+  <si>
+    <t>rqwskxphikhxvilf</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Angelagrahamd2@gmail.com</t>
+  </si>
+  <si>
+    <t>pzwlnpwgefuwfhll</t>
+  </si>
+  <si>
+    <t>193.243.189.88:54895</t>
+  </si>
+  <si>
+    <t>6mzL884tfGrvkN8T</t>
+  </si>
+  <si>
+    <t>PDD3ZP27f9uXUYdE</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>Bishop</t>
+  </si>
+  <si>
+    <t>Helenbishopc4@gmail.com</t>
+  </si>
+  <si>
+    <t>bovaflmxitcpukai</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Lisajordanc4@gmail.com</t>
+  </si>
+  <si>
+    <t>uvbhattfkpzjorip</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>Perry</t>
+  </si>
+  <si>
+    <t>Francesperryv4@gmail.com</t>
+  </si>
+  <si>
+    <t>kwnckmsdzwveuoga</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>Susanrobinsonc5@gmail.com</t>
+  </si>
+  <si>
+    <t>hpdfvjjmolsxkcab</t>
+  </si>
+  <si>
+    <t>Kathryn</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>Kathrynwardd4@gmail.com</t>
+  </si>
+  <si>
+    <t>gdtqndfnjalkbfzr</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Virginiajenkinsc4@gmail.com</t>
+  </si>
+  <si>
+    <t>dxlibiuqqqwiisho</t>
+  </si>
+  <si>
+    <t>Oliviajenkinsc4@gmail.com</t>
+  </si>
+  <si>
+    <t>vkrptypgielfiycv</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>Alicebanksy4@gmail.com</t>
+  </si>
+  <si>
+    <t>inhzzttzmtgvivvz</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Katherinebradleyd4@gmail.com</t>
+  </si>
+  <si>
+    <t>vkjcnqxrbgtxoowm</t>
+  </si>
+  <si>
+    <t>193.243.189.88:64544</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>elizabethwilsonp4@gmail.com</t>
+  </si>
+  <si>
+    <t>hwmipwtyzvfhtldj</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Sandoval</t>
+  </si>
+  <si>
+    <t>sarasandovalq2@gmail.com</t>
+  </si>
+  <si>
+    <t>nbsddwyhmebuzwqy</t>
+  </si>
+  <si>
+    <t>Carr</t>
+  </si>
+  <si>
+    <t>oliviacarrq2@gmail.com</t>
+  </si>
+  <si>
+    <t>oucfpvsjxqaujbke</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>carolcarrollp4@gmail.com</t>
+  </si>
+  <si>
+    <t>mvpbmugsnygnomyv</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Garrett</t>
+  </si>
+  <si>
+    <t>rebeccagarrettp6@gmail.com</t>
+  </si>
+  <si>
+    <t>wgxnoodsnedbbkcu</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Lane</t>
+  </si>
+  <si>
+    <t>deniselanep5@gmail.com</t>
+  </si>
+  <si>
+    <t>ciyzxpvxcatpomns</t>
+  </si>
+  <si>
+    <t>Deborah</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>deborahblackp5@gmail.com</t>
+  </si>
+  <si>
+    <t>vrshuummcymwujuf</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>jessicacastrop3@gmail.com</t>
+  </si>
+  <si>
+    <t>gvetrxupnsxhjbfr</t>
+  </si>
+  <si>
+    <t>Marilyn</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>marilynaustinp4@gmail.com</t>
+  </si>
+  <si>
+    <t>yqohmxuxaukauhti</t>
+  </si>
+  <si>
+    <t>193.243.189.88:64751</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1333,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G38"/>
+      <selection activeCell="D3" sqref="A1:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1483,853 +1363,853 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="G24" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G28" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G32" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G33" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G34" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="G35" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="C36" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G36" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="D37" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G37" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="C38" t="s">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>49</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random number of emails in smtp send
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,12 +226,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -414,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -529,66 +523,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -634,20 +568,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1003,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G24"/>
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1102,186 +1024,6 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added checkboxes for white list , space encoding, test email will be cached from now on
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1E4B3C-149C-45C7-B1CF-5AC234A51853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group_b" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -103,12 +104,66 @@
   </si>
   <si>
     <t>102.223.180.88:4000</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>john.snow42@outlook.hu</t>
+  </si>
+  <si>
+    <t>Whateverpass0*</t>
+  </si>
+  <si>
+    <t>81.28.96.148:4000</t>
+  </si>
+  <si>
+    <t>i0BdGW79w6Oo</t>
+  </si>
+  <si>
+    <t>5Ao37R1ry6bc</t>
+  </si>
+  <si>
+    <t>Louise</t>
+  </si>
+  <si>
+    <t>Deforge</t>
+  </si>
+  <si>
+    <t>saidunuhu579@gmail.com</t>
+  </si>
+  <si>
+    <t>ujemlxfzbgwnkzpd</t>
+  </si>
+  <si>
+    <t>185.125.171.221:4021</t>
+  </si>
+  <si>
+    <t>2JjU2izT4rk1tGb</t>
+  </si>
+  <si>
+    <t>bEjmSK36Ma4C36t</t>
+  </si>
+  <si>
+    <t>Janice</t>
+  </si>
+  <si>
+    <t>Holley</t>
+  </si>
+  <si>
+    <t>lithbello60@gmail.com</t>
+  </si>
+  <si>
+    <t>wrddcsqmfqdkqkrx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -942,23 +997,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +1036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1004,7 +1059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1027,7 +1082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1048,6 +1103,75 @@
       </c>
       <c r="G4" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed whitelist, name and test email caching
</commit_message>
<xml_diff>
--- a/database/group_b.xlsx
+++ b/database/group_b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1E4B3C-149C-45C7-B1CF-5AC234A51853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5404FCC3-2CFC-4046-82F7-F33C65143162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -158,6 +158,27 @@
   </si>
   <si>
     <t>wrddcsqmfqdkqkrx</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>walteru6_newportgw@outlook.com</t>
+  </si>
+  <si>
+    <t>wba18Hq1BbNr5xd</t>
+  </si>
+  <si>
+    <t>81.28.96.40:4004</t>
+  </si>
+  <si>
+    <t>PJ5C8sm37i4b</t>
+  </si>
+  <si>
+    <t>56gRMx51KSrg</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,131 +1059,131 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1171,6 +1192,29 @@
         <v>40</v>
       </c>
       <c r="G7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>